<commit_message>
data provider in add client with assert
</commit_message>
<xml_diff>
--- a/Data/data.xlsx
+++ b/Data/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>surname</t>
   </si>
@@ -111,9 +111,6 @@
     <t>567-999-7457</t>
   </si>
   <si>
-    <t>amol</t>
-  </si>
-  <si>
     <t>ujagare</t>
   </si>
   <si>
@@ -124,6 +121,24 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>expected result</t>
+  </si>
+  <si>
+    <t>Client already exists!</t>
+  </si>
+  <si>
+    <t>amol1235</t>
+  </si>
+  <si>
+    <t>Record successfully created</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'alert')]</t>
+  </si>
+  <si>
+    <t>xpath of actual result</t>
   </si>
 </sst>
 </file>
@@ -471,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -483,9 +498,12 @@
     <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -540,8 +558,14 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75">
+    <row r="2" spans="1:20" ht="15.75">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -555,7 +579,7 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -570,7 +594,7 @@
         <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>23</v>
@@ -596,13 +620,19 @@
       <c r="R2">
         <v>3434</v>
       </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75">
+    <row r="3" spans="1:20" ht="15.75">
       <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -611,7 +641,7 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -626,7 +656,7 @@
         <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>29</v>
@@ -651,6 +681,12 @@
       </c>
       <c r="R3">
         <v>3435</v>
+      </c>
+      <c r="S3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Database testing part 1
</commit_message>
<xml_diff>
--- a/Data/data.xlsx
+++ b/Data/data.xlsx
@@ -99,9 +99,6 @@
     <t>www.xyz</t>
   </si>
   <si>
-    <t>praful</t>
-  </si>
-  <si>
     <t>ghodake</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Client already exists!</t>
   </si>
   <si>
-    <t>amol1235</t>
-  </si>
-  <si>
     <t>Record successfully created</t>
   </si>
   <si>
@@ -139,6 +133,12 @@
   </si>
   <si>
     <t>xpath of actual result</t>
+  </si>
+  <si>
+    <t>ravi</t>
+  </si>
+  <si>
+    <t>vipin</t>
   </si>
 </sst>
 </file>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -559,18 +559,18 @@
         <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -579,7 +579,7 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -594,7 +594,7 @@
         <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>23</v>
@@ -621,18 +621,18 @@
         <v>3434</v>
       </c>
       <c r="S2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -641,7 +641,7 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -656,13 +656,13 @@
         <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
         <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
       </c>
       <c r="M3">
         <v>45679</v>
@@ -683,10 +683,10 @@
         <v>3435</v>
       </c>
       <c r="S3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="T3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Database testing part 3
</commit_message>
<xml_diff>
--- a/Data/data.xlsx
+++ b/Data/data.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="17175" windowHeight="6930"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="17175" windowHeight="6930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Database testing" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>surname</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>vipin</t>
+  </si>
+  <si>
+    <t>ajay3</t>
   </si>
 </sst>
 </file>
@@ -488,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -703,12 +706,131 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2">
+        <v>8827</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2">
+        <v>45678</v>
+      </c>
+      <c r="N2">
+        <v>76543</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2">
+        <v>434</v>
+      </c>
+      <c r="R2">
+        <v>3434</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P2" r:id="rId1"/>
+    <hyperlink ref="O2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>